<commit_message>
Submitted week 2 timesheet
</commit_message>
<xml_diff>
--- a/Moore-Heather-timesheet.xlsx
+++ b/Moore-Heather-timesheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="220" windowWidth="24560" windowHeight="17060" tabRatio="560"/>
+    <workbookView xWindow="-100" yWindow="-80" windowWidth="24560" windowHeight="17060" tabRatio="560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="14">
   <si>
     <t>Weekley Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,17 +80,19 @@
     <t>Met with client to go over details for website</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Created WordPress mockup for peer presentation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Moved WP mockup to live server, prepared for peer presentation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
@@ -183,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -212,6 +214,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,7 +551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -663,7 +666,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -725,7 +727,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -791,7 +793,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -857,7 +859,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -923,7 +925,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -989,7 +991,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -1055,7 +1057,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -1121,7 +1123,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -1141,13 +1143,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="44.28515625" customWidth="1"/>
+    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1168,13 +1170,47 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1">
+      <c r="A2" s="5">
+        <v>41654</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1">
+      <c r="A3" s="5">
+        <v>41655</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
@@ -1183,7 +1219,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 1'!E21</f>
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -1249,7 +1285,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 2'!E21</f>
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -1315,7 +1351,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 3'!E21</f>
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -1381,7 +1417,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 4'!E21</f>
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -1447,7 +1483,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 5'!E21</f>
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -1513,7 +1549,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 6'!E21</f>
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -1579,7 +1615,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 7'!E21</f>
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>
@@ -1645,7 +1681,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated timesheet week 3
</commit_message>
<xml_diff>
--- a/Moore-Heather-timesheet.xlsx
+++ b/Moore-Heather-timesheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="-80" windowWidth="24560" windowHeight="17060" tabRatio="560" activeTab="1"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="17300" tabRatio="560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="16">
   <si>
     <t>Weekley Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,6 +87,13 @@
   <si>
     <t>Moved WP mockup to live server, prepared for peer presentation</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Presented my project idea to the class, got feedback, gave feedback to other students on their projects</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compared different online payment services, created databases for laravel, migrated databases, completed ERD, began project description</t>
   </si>
 </sst>
 </file>
@@ -185,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -215,6 +222,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,7 +737,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
-        <v>8.5</v>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>
@@ -793,7 +803,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
-        <v>8.5</v>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>
@@ -859,7 +869,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>8.5</v>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>
@@ -925,7 +935,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>8.5</v>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>
@@ -991,7 +1001,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>8.5</v>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>
@@ -1057,7 +1067,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>8.5</v>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>
@@ -1123,7 +1133,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>8.5</v>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>
@@ -1143,7 +1153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1223,7 +1233,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1243,17 +1252,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
   <cols>
     <col min="4" max="4" width="44.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
+    <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1270,22 +1279,56 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="4:5" ht="18" customHeight="1">
+    <row r="2" spans="1:5" ht="26">
+      <c r="A2" s="5">
+        <v>41661</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="39">
+      <c r="A3" s="5">
+        <v>41663</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="4:5" ht="18" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E21">
         <f>E20+'Week 2'!E21</f>
-        <v>8.5</v>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>
@@ -1351,7 +1394,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 3'!E21</f>
-        <v>8.5</v>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>
@@ -1417,7 +1460,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 4'!E21</f>
-        <v>8.5</v>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>
@@ -1483,7 +1526,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 5'!E21</f>
-        <v>8.5</v>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>
@@ -1549,7 +1592,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 6'!E21</f>
-        <v>8.5</v>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>
@@ -1615,7 +1658,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 7'!E21</f>
-        <v>8.5</v>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>
@@ -1681,7 +1724,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>
-        <v>8.5</v>
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated timesheet week 4
</commit_message>
<xml_diff>
--- a/Moore-Heather-timesheet.xlsx
+++ b/Moore-Heather-timesheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="17300" tabRatio="560" activeTab="2"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="17300" tabRatio="560" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="20">
   <si>
     <t>Weekley Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,6 +94,22 @@
   </si>
   <si>
     <t>Compared different online payment services, created databases for laravel, migrated databases, completed ERD, began project description</t>
+  </si>
+  <si>
+    <t>Researched how to deploy Laravel project to shared server</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Researched Deployer to upload Laravel to shared server</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished project description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contacted SiteGround support and adjusted settings to get Laravel project deployed live</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -737,11 +753,10 @@
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
-        <v>12.5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -803,11 +818,10 @@
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
-        <v>12.5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -869,11 +883,10 @@
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>12.5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -935,11 +948,10 @@
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>12.5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1001,11 +1013,10 @@
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>12.5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1067,11 +1078,10 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>12.5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1133,11 +1143,10 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>12.5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1252,7 +1261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1332,7 +1341,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1352,17 +1360,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
   <cols>
     <col min="4" max="4" width="44.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
+    <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1379,26 +1387,93 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="4:5" ht="18" customHeight="1">
+    <row r="2" spans="1:5">
+      <c r="A2" s="5">
+        <v>41666</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="5">
+        <v>41667</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="5">
+        <v>41668</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="26">
+      <c r="A5" s="5">
+        <v>41668</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="4:5" ht="18" customHeight="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E21">
         <f>E20+'Week 3'!E21</f>
-        <v>12.5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1460,11 +1535,10 @@
       </c>
       <c r="E21">
         <f>E20+'Week 4'!E21</f>
-        <v>12.5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1526,11 +1600,10 @@
       </c>
       <c r="E21">
         <f>E20+'Week 5'!E21</f>
-        <v>12.5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1592,11 +1665,10 @@
       </c>
       <c r="E21">
         <f>E20+'Week 6'!E21</f>
-        <v>12.5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1658,11 +1730,10 @@
       </c>
       <c r="E21">
         <f>E20+'Week 7'!E21</f>
-        <v>12.5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1724,11 +1795,10 @@
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>
-        <v>12.5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updated ERD and timeline week 5
</commit_message>
<xml_diff>
--- a/Moore-Heather-timesheet.xlsx
+++ b/Moore-Heather-timesheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="17300" tabRatio="560" activeTab="3"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="17300" tabRatio="560" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="22">
   <si>
     <t>Weekley Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -113,6 +113,10 @@
   </si>
   <si>
     <t>Database presentation with Brenda McFarland, updated Alchemortem database ERD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added foreign keys to tables, migrated tables to db</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -757,10 +761,11 @@
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -822,7 +827,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -887,7 +892,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -952,7 +957,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1017,7 +1022,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1082,7 +1087,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1147,7 +1152,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1246,6 +1251,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1345,6 +1351,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1364,7 +1371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1495,6 +1502,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1514,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" customHeight="1"/>
@@ -1541,13 +1549,30 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1">
+      <c r="A2" s="5">
+        <v>41675</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
@@ -1556,10 +1581,11 @@
       </c>
       <c r="E21">
         <f>E20+'Week 4'!E21</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1621,10 +1647,11 @@
       </c>
       <c r="E21">
         <f>E20+'Week 5'!E21</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1686,10 +1713,11 @@
       </c>
       <c r="E21">
         <f>E20+'Week 6'!E21</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1751,10 +1779,11 @@
       </c>
       <c r="E21">
         <f>E20+'Week 7'!E21</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1816,10 +1845,11 @@
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updated timesheet week 6
</commit_message>
<xml_diff>
--- a/Moore-Heather-timesheet.xlsx
+++ b/Moore-Heather-timesheet.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="23">
   <si>
     <t>Weekley Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -117,6 +117,10 @@
   </si>
   <si>
     <t>Added foreign keys to tables, migrated tables to db</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created sql database dump for alchemortem, created master layout for laravel application</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -761,11 +765,10 @@
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -827,7 +830,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -892,7 +895,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -957,7 +960,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1022,7 +1025,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1087,7 +1090,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1152,7 +1155,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1251,7 +1254,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1351,7 +1353,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1502,7 +1503,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1523,16 +1523,16 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
   <cols>
     <col min="4" max="4" width="44.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
+    <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" customHeight="1">
+    <row r="2" spans="1:5">
       <c r="A2" s="5">
         <v>41675</v>
       </c>
@@ -1566,26 +1566,42 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="4:5" ht="18" customHeight="1">
+    <row r="3" spans="1:5" ht="26">
+      <c r="A3" s="5">
+        <v>41677</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="4:5" ht="18" customHeight="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E21">
         <f>E20+'Week 4'!E21</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1647,11 +1663,10 @@
       </c>
       <c r="E21">
         <f>E20+'Week 5'!E21</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1713,11 +1728,10 @@
       </c>
       <c r="E21">
         <f>E20+'Week 6'!E21</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1779,11 +1793,10 @@
       </c>
       <c r="E21">
         <f>E20+'Week 7'!E21</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1845,11 +1858,10 @@
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Renamed product images, updated timesheet week 6
</commit_message>
<xml_diff>
--- a/Moore-Heather-timesheet.xlsx
+++ b/Moore-Heather-timesheet.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="28">
   <si>
     <t>Finished master layout, started index page</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -137,6 +137,10 @@
   </si>
   <si>
     <t>Finished editing product images, started master layout and product page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Uploaded product images, created states lookup table, modified table relationships, resolved terminal issue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -720,6 +724,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -781,10 +786,11 @@
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
-        <v>30.5</v>
+        <v>32.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -846,10 +852,11 @@
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
-        <v>30.5</v>
+        <v>32.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -911,10 +918,11 @@
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>30.5</v>
+        <v>32.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -976,10 +984,11 @@
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>30.5</v>
+        <v>32.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1041,10 +1050,11 @@
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>30.5</v>
+        <v>32.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1106,10 +1116,11 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>30.5</v>
+        <v>32.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1171,10 +1182,11 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>30.5</v>
+        <v>32.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1370,6 +1382,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1520,6 +1533,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1619,6 +1633,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1639,7 +1654,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" customHeight="1"/>
@@ -1733,13 +1748,30 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:5" ht="26">
+      <c r="A6" s="5">
+        <v>41684</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>4.5</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
@@ -1748,10 +1780,11 @@
       </c>
       <c r="E21">
         <f>E20+'Week 5'!E21</f>
-        <v>30.5</v>
+        <v>32.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1813,10 +1846,11 @@
       </c>
       <c r="E21">
         <f>E20+'Week 6'!E21</f>
-        <v>30.5</v>
+        <v>32.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1878,10 +1912,11 @@
       </c>
       <c r="E21">
         <f>E20+'Week 7'!E21</f>
-        <v>30.5</v>
+        <v>32.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1943,10 +1978,11 @@
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>
-        <v>30.5</v>
+        <v>32.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Submitted timesheet week 6
</commit_message>
<xml_diff>
--- a/Moore-Heather-timesheet.xlsx
+++ b/Moore-Heather-timesheet.xlsx
@@ -34,7 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="30">
+  <si>
+    <t>Seeded states table, images table, payment table, role table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seeded products table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Finished master layout, started index page</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -622,19 +630,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26">
@@ -648,7 +656,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -665,7 +673,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>0.5</v>
@@ -682,7 +690,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -699,7 +707,7 @@
         <v>0.5</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -707,7 +715,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="10" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -716,7 +724,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="10" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <f>E20</f>
@@ -756,24 +764,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -782,11 +790,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
-        <v>32.5</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -822,24 +830,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -848,11 +856,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
-        <v>32.5</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -888,24 +896,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -914,11 +922,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>32.5</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -954,24 +962,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -980,11 +988,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>32.5</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1020,24 +1028,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1046,11 +1054,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>32.5</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1086,24 +1094,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1112,11 +1120,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>32.5</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1152,24 +1160,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1178,11 +1186,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>32.5</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1214,19 +1222,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -1240,7 +1248,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1257,7 +1265,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1265,7 +1273,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1274,7 +1282,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <f>E20+'Week 1'!E21</f>
@@ -1314,19 +1322,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26">
@@ -1340,7 +1348,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1357,7 +1365,7 @@
         <v>0.5</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1365,7 +1373,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1374,7 +1382,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <f>E20+'Week 2'!E21</f>
@@ -1414,19 +1422,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1440,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1457,7 +1465,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E3">
         <v>2.5</v>
@@ -1474,7 +1482,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1491,7 +1499,7 @@
         <v>0.875</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1508,7 +1516,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1516,7 +1524,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1525,7 +1533,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <f>E20+'Week 3'!E21</f>
@@ -1565,19 +1573,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1591,7 +1599,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1608,7 +1616,7 @@
         <v>0.5</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1616,7 +1624,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1625,7 +1633,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <f>E20+'Week 4'!E21</f>
@@ -1654,7 +1662,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" customHeight="1"/>
@@ -1665,19 +1673,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -1691,7 +1699,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E2">
         <v>0.5</v>
@@ -1708,7 +1716,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1725,7 +1733,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1742,7 +1750,7 @@
         <v>0.875</v>
       </c>
       <c r="D5" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1759,28 +1767,62 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
     </row>
+    <row r="7" spans="1:5" ht="26">
+      <c r="A7" s="5">
+        <v>41684</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" customHeight="1">
+      <c r="A8" s="5">
+        <v>41684</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>6.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <f>E20+'Week 5'!E21</f>
-        <v>32.5</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1816,24 +1858,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1842,11 +1884,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <f>E20+'Week 6'!E21</f>
-        <v>32.5</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1882,24 +1924,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1908,11 +1950,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <f>E20+'Week 7'!E21</f>
-        <v>32.5</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1948,24 +1990,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1974,11 +2016,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>
-        <v>32.5</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Submitted timesheet week 7 and phase 3
</commit_message>
<xml_diff>
--- a/Moore-Heather-timesheet.xlsx
+++ b/Moore-Heather-timesheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="17300" tabRatio="560" activeTab="5"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="17300" tabRatio="560" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="32">
+  <si>
+    <t>Successfully displayed database values for product table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Worked on product/image relationship</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Seeded states table, images table, payment table, role table</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -630,19 +638,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26">
@@ -656,7 +664,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -673,7 +681,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>0.5</v>
@@ -690,7 +698,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -707,7 +715,7 @@
         <v>0.5</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -715,7 +723,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -724,7 +732,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <f>E20</f>
@@ -732,7 +740,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -764,24 +771,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -790,11 +797,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
-        <v>37</v>
+        <v>42.5</v>
       </c>
     </row>
   </sheetData>
@@ -830,24 +837,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -856,11 +863,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
-        <v>37</v>
+        <v>42.5</v>
       </c>
     </row>
   </sheetData>
@@ -896,24 +903,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -922,11 +929,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>37</v>
+        <v>42.5</v>
       </c>
     </row>
   </sheetData>
@@ -962,24 +969,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -988,11 +995,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>37</v>
+        <v>42.5</v>
       </c>
     </row>
   </sheetData>
@@ -1028,24 +1035,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1054,11 +1061,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>37</v>
+        <v>42.5</v>
       </c>
     </row>
   </sheetData>
@@ -1094,24 +1101,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1120,11 +1127,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>37</v>
+        <v>42.5</v>
       </c>
     </row>
   </sheetData>
@@ -1160,24 +1167,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1186,11 +1193,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>37</v>
+        <v>42.5</v>
       </c>
     </row>
   </sheetData>
@@ -1222,19 +1229,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -1248,7 +1255,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1265,7 +1272,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1273,7 +1280,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1282,7 +1289,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <f>E20+'Week 1'!E21</f>
@@ -1322,19 +1329,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26">
@@ -1348,7 +1355,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1365,7 +1372,7 @@
         <v>0.5</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1373,7 +1380,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1382,7 +1389,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <f>E20+'Week 2'!E21</f>
@@ -1422,19 +1429,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1448,7 +1455,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1465,7 +1472,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3">
         <v>2.5</v>
@@ -1482,7 +1489,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1499,7 +1506,7 @@
         <v>0.875</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1516,7 +1523,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1524,7 +1531,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1533,7 +1540,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <f>E20+'Week 3'!E21</f>
@@ -1573,19 +1580,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1599,7 +1606,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1616,7 +1623,7 @@
         <v>0.5</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1624,7 +1631,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1633,7 +1640,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <f>E20+'Week 4'!E21</f>
@@ -1661,7 +1668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1673,19 +1680,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -1699,7 +1706,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E2">
         <v>0.5</v>
@@ -1716,7 +1723,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1733,7 +1740,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1750,7 +1757,7 @@
         <v>0.875</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1767,7 +1774,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1784,7 +1791,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <v>2.5</v>
@@ -1801,7 +1808,7 @@
         <v>0.95833333333333337</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -1809,7 +1816,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1818,7 +1825,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <f>E20+'Week 5'!E21</f>
@@ -1846,8 +1853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" customHeight="1"/>
@@ -1858,37 +1865,88 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1">
+      <c r="A2" s="5">
+        <v>41689</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1">
+      <c r="A3" s="5">
+        <v>41690</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1">
+      <c r="A4" s="5">
+        <v>41691</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <f>E20+'Week 6'!E21</f>
-        <v>37</v>
+        <v>42.5</v>
       </c>
     </row>
   </sheetData>
@@ -1924,24 +1982,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1950,11 +2008,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <f>E20+'Week 7'!E21</f>
-        <v>37</v>
+        <v>42.5</v>
       </c>
     </row>
   </sheetData>
@@ -1990,24 +2048,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -2016,11 +2074,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>
-        <v>37</v>
+        <v>42.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Submitted timeline week 8
</commit_message>
<xml_diff>
--- a/Moore-Heather-timesheet.xlsx
+++ b/Moore-Heather-timesheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="17300" tabRatio="560" activeTab="6"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="17300" tabRatio="560" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="39">
+  <si>
+    <t>Reviewed capstone project timeline, went over rubric, overview of syllabus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brainstormed ideas for Capstone project, setup meeting with website client to discuss details for project</t>
+  </si>
+  <si>
+    <t>Compiled list of details to get from client</t>
+  </si>
+  <si>
+    <t>Met with client to go over details for website</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created WordPress mockup for peer presentation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Moved WP mockup to live server, prepared for peer presentation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Presented my project idea to the class, got feedback, gave feedback to other students on their projects</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compared different online payment services, created databases for laravel, migrated databases, completed ERD, began project description</t>
+  </si>
+  <si>
+    <t>Researched how to deploy Laravel project to shared server</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Researched Deployer to upload Laravel to shared server</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished project description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contacted SiteGround support and adjusted settings to get Laravel project deployed live</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Database presentation with Brenda McFarland, updated Alchemortem database ERD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added foreign keys to tables, migrated tables to db</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created sql database dump for alchemortem, created master layout for laravel application</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meet with client to get product info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Photographed and started editing product images</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished editing product images, started master layout and product page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Successful add to cart, view cart, and started on checkout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Uploaded product images, created states lookup table, modified table relationships, resolved terminal issue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created dropdown sign in on navbar, adjusted CSS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created sign up page, linked page in navigation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created and tested form to add new user which redirects to index, added roles and policies to users, created "manage users" page for admin role</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created sign in views and functions in UserController</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sign up auto login, redirects to user account, authorization on guest (cannot view account unless logged in), created cart model to add products to cart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added images to products table, successful display of images with products on products page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Successfully displayed database values for product table</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -85,79 +186,6 @@
   </si>
   <si>
     <t>Weekly Total</t>
-  </si>
-  <si>
-    <t>Reviewed capstone project timeline, went over rubric, overview of syllabus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Brainstormed ideas for Capstone project, setup meeting with website client to discuss details for project</t>
-  </si>
-  <si>
-    <t>Compiled list of details to get from client</t>
-  </si>
-  <si>
-    <t>Met with client to go over details for website</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Created WordPress mockup for peer presentation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Moved WP mockup to live server, prepared for peer presentation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Presented my project idea to the class, got feedback, gave feedback to other students on their projects</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Compared different online payment services, created databases for laravel, migrated databases, completed ERD, began project description</t>
-  </si>
-  <si>
-    <t>Researched how to deploy Laravel project to shared server</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Researched Deployer to upload Laravel to shared server</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Finished project description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Contacted SiteGround support and adjusted settings to get Laravel project deployed live</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Database presentation with Brenda McFarland, updated Alchemortem database ERD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Added foreign keys to tables, migrated tables to db</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Created sql database dump for alchemortem, created master layout for laravel application</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Meet with client to get product info</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Photographed and started editing product images</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Finished editing product images, started master layout and product page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Uploaded product images, created states lookup table, modified table relationships, resolved terminal issue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -256,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -289,6 +317,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,19 +671,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26">
@@ -664,7 +697,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -681,7 +714,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0.5</v>
@@ -698,7 +731,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -715,7 +748,7 @@
         <v>0.5</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -723,7 +756,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="10" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -732,7 +765,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="10" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20</f>
@@ -771,24 +804,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -797,15 +830,14 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
-        <v>42.5</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -837,24 +869,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -863,15 +895,14 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
-        <v>42.5</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -903,24 +934,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -929,15 +960,14 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>42.5</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -969,24 +999,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -995,15 +1025,14 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>42.5</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1035,24 +1064,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1061,15 +1090,14 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>42.5</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1101,24 +1129,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1127,15 +1155,14 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>42.5</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1167,24 +1194,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1193,15 +1220,14 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>42.5</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1229,19 +1255,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -1255,7 +1281,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1272,7 +1298,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1280,7 +1306,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1289,7 +1315,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 1'!E21</f>
@@ -1297,7 +1323,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1329,19 +1354,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26">
@@ -1355,7 +1380,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1372,7 +1397,7 @@
         <v>0.5</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1380,7 +1405,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1389,7 +1414,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 2'!E21</f>
@@ -1397,7 +1422,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1429,19 +1453,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1455,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1472,7 +1496,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>2.5</v>
@@ -1489,7 +1513,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1506,7 +1530,7 @@
         <v>0.875</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1523,7 +1547,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1531,7 +1555,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1540,7 +1564,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 3'!E21</f>
@@ -1548,7 +1572,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1580,19 +1603,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1606,7 +1629,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1623,7 +1646,7 @@
         <v>0.5</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1631,7 +1654,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1640,7 +1663,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 4'!E21</f>
@@ -1648,7 +1671,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1680,19 +1702,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -1706,7 +1728,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <v>0.5</v>
@@ -1723,7 +1745,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1740,7 +1762,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1757,7 +1779,7 @@
         <v>0.875</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1774,7 +1796,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1791,7 +1813,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E7">
         <v>2.5</v>
@@ -1808,7 +1830,7 @@
         <v>0.95833333333333337</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -1816,7 +1838,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1825,7 +1847,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 5'!E21</f>
@@ -1833,7 +1855,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1853,7 +1874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1865,19 +1886,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -1891,7 +1912,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1908,7 +1929,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="E3">
         <v>1.5</v>
@@ -1925,7 +1946,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1933,7 +1954,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1942,7 +1963,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 6'!E21</f>
@@ -1950,7 +1971,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1970,53 +1990,172 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" customHeight="1"/>
   <cols>
+    <col min="1" max="1" width="11" style="14"/>
     <col min="4" max="4" width="44.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
+      <c r="A1" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1">
+      <c r="A2" s="14">
+        <v>41693</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1">
+      <c r="A3" s="14">
+        <v>41694</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="39">
+      <c r="A4" s="14">
+        <v>41695</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" customHeight="1">
+      <c r="A5" s="14">
+        <v>41695</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.6875</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="39">
+      <c r="A6" s="14">
+        <v>41696</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="26">
+      <c r="A7" s="14">
+        <v>41696</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" customHeight="1">
+      <c r="A8" s="14">
+        <v>41698</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 7'!E21</f>
-        <v>42.5</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2048,24 +2187,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -2074,15 +2213,14 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>
-        <v>42.5</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Submitted timesheet week 9
</commit_message>
<xml_diff>
--- a/Moore-Heather-timesheet.xlsx
+++ b/Moore-Heather-timesheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="17300" tabRatio="560" activeTab="7"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="17300" tabRatio="560" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,154 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="47">
+  <si>
+    <t>Worked on deleting items from cart and updating cart data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added successful checkout page, successful checkout orders store in database with logged in user relationship</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished project description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contacted SiteGround support and adjusted settings to get Laravel project deployed live</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Database presentation with Brenda McFarland, updated Alchemortem database ERD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added foreign keys to tables, migrated tables to db</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created sql database dump for alchemortem, created master layout for laravel application</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meet with client to get product info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Photographed and started editing product images</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished editing product images, started master layout and product page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Successful add to cart, view cart, and started on checkout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Uploaded product images, created states lookup table, modified table relationships, resolved terminal issue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created dropdown sign in on navbar, adjusted CSS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created sign up page, linked page in navigation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created and tested form to add new user which redirects to index, added roles and policies to users, created "manage users" page for admin role</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created sign in views and functions in UserController</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Forced user login to checkout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created single item view with all product details, updated edit product page with select attribute for status, updated edit user page with select attribute for role</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sign up auto login, redirects to user account, authorization on guest (cannot view account unless logged in), created cart model to add products to cart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added images to products table, successful display of images with products on products page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Successfully displayed database values for product table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Worked on product/image relationship</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seeded states table, images table, payment table, role table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seeded products table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished master layout, started index page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weekley Total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Project Total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Start Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>End Time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Hours</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weekly Total</t>
+  </si>
+  <si>
+    <t>Created and tested "Add product" page, created admin view to show all products, created "Edit user" button and form, Created and tested "Delete user" button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Successful edit user, edit product, and delete product, created FAQ page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Worked on profile page, created checkout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up checkout to Stripe, successful test charges from website to Stripe account</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Reviewed capstone project timeline, went over rubric, overview of syllabus</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,121 +218,6 @@
   <si>
     <t>Researched Deployer to upload Laravel to shared server</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Finished project description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Contacted SiteGround support and adjusted settings to get Laravel project deployed live</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Database presentation with Brenda McFarland, updated Alchemortem database ERD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Added foreign keys to tables, migrated tables to db</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Created sql database dump for alchemortem, created master layout for laravel application</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Meet with client to get product info</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Photographed and started editing product images</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Finished editing product images, started master layout and product page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Successful add to cart, view cart, and started on checkout</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Uploaded product images, created states lookup table, modified table relationships, resolved terminal issue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Created dropdown sign in on navbar, adjusted CSS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Created sign up page, linked page in navigation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Created and tested form to add new user which redirects to index, added roles and policies to users, created "manage users" page for admin role</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Created sign in views and functions in UserController</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sign up auto login, redirects to user account, authorization on guest (cannot view account unless logged in), created cart model to add products to cart</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Added images to products table, successful display of images with products on products page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Successfully displayed database values for product table</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Worked on product/image relationship</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Seeded states table, images table, payment table, role table</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Seeded products table</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Finished master layout, started index page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Weekley Total</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Project Total</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Start Time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>End Time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total Hours</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Weekly Total</t>
   </si>
 </sst>
 </file>
@@ -671,19 +703,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26">
@@ -697,7 +729,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -714,7 +746,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="E3">
         <v>0.5</v>
@@ -731,7 +763,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -748,7 +780,7 @@
         <v>0.5</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -756,7 +788,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="10" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -765,7 +797,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="10" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E21">
         <f>E20</f>
@@ -792,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" customHeight="1"/>
@@ -804,40 +836,106 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1">
+      <c r="A2" s="14">
+        <v>41708</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.9375</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="39">
+      <c r="A3" s="14">
+        <v>41709</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1">
+      <c r="A4" s="14">
+        <v>41710</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="26">
+      <c r="A5" s="14">
+        <v>41711</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
-        <v>54</v>
+        <v>67.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -869,24 +967,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -895,14 +993,15 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
-        <v>54</v>
+        <v>67.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -934,24 +1033,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -960,14 +1059,15 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>54</v>
+        <v>67.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -999,24 +1099,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1025,14 +1125,15 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>54</v>
+        <v>67.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1064,24 +1165,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1090,14 +1191,15 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>54</v>
+        <v>67.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1129,24 +1231,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1155,14 +1257,15 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>54</v>
+        <v>67.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1194,24 +1297,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1220,14 +1323,15 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>54</v>
+        <v>67.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1255,19 +1359,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -1281,7 +1385,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1298,7 +1402,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1306,7 +1410,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1315,7 +1419,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E21">
         <f>E20+'Week 1'!E21</f>
@@ -1354,19 +1458,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26">
@@ -1380,7 +1484,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1397,7 +1501,7 @@
         <v>0.5</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1405,7 +1509,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1414,7 +1518,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E21">
         <f>E20+'Week 2'!E21</f>
@@ -1453,19 +1557,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1479,7 +1583,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1496,7 +1600,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="E3">
         <v>2.5</v>
@@ -1513,7 +1617,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1530,7 +1634,7 @@
         <v>0.875</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1547,7 +1651,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1555,7 +1659,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1564,7 +1668,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E21">
         <f>E20+'Week 3'!E21</f>
@@ -1603,19 +1707,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1629,7 +1733,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1646,7 +1750,7 @@
         <v>0.5</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1654,7 +1758,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1663,7 +1767,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E21">
         <f>E20+'Week 4'!E21</f>
@@ -1702,19 +1806,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -1728,7 +1832,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E2">
         <v>0.5</v>
@@ -1745,7 +1849,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1762,7 +1866,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1779,7 +1883,7 @@
         <v>0.875</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1796,7 +1900,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1813,7 +1917,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E7">
         <v>2.5</v>
@@ -1830,7 +1934,7 @@
         <v>0.95833333333333337</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -1838,7 +1942,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1847,7 +1951,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E21">
         <f>E20+'Week 5'!E21</f>
@@ -1886,19 +1990,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -1912,7 +2016,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1929,7 +2033,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>1.5</v>
@@ -1946,7 +2050,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1954,7 +2058,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1963,7 +2067,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E21">
         <f>E20+'Week 6'!E21</f>
@@ -1990,7 +2094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -2003,19 +2107,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -2029,7 +2133,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -2046,7 +2150,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -2063,7 +2167,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2080,7 +2184,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2097,7 +2201,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -2114,7 +2218,7 @@
         <v>0.22916666666666666</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E7">
         <v>1.5</v>
@@ -2131,7 +2235,7 @@
         <v>0.5</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -2139,7 +2243,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -2148,7 +2252,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E21">
         <f>E20+'Week 7'!E21</f>
@@ -2156,6 +2260,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2176,7 +2281,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" customHeight="1"/>
@@ -2187,40 +2292,109 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="39">
+      <c r="A2" s="14">
+        <v>41703</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.9375</v>
+      </c>
+      <c r="C2" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="26">
+      <c r="A3" s="14">
+        <v>41704</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.6875</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1">
+      <c r="A4" s="14">
+        <v>41705</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D4" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="26">
+      <c r="A5" s="14">
+        <v>41706</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>36</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>
-        <v>54</v>
+        <v>62.5</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Submitted timesheet week 11
</commit_message>
<xml_diff>
--- a/Moore-Heather-timesheet.xlsx
+++ b/Moore-Heather-timesheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="17300" tabRatio="560" activeTab="9"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="17300" tabRatio="560" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -34,13 +34,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="53">
   <si>
     <t>Worked on deleting items from cart and updating cart data</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Added successful checkout page, successful checkout orders store in database with logged in user relationship</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created and tested view to display all orders of logged in user, added reduce, increase, and remove links on cart view, created view to display user info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Worked on restricting admin views from regular users</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added and tested user info update button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adjusted CSS on all pages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added incorrect password error message, created and tested password reset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Worked on CSS and resposiveness</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -703,19 +727,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26">
@@ -729,7 +753,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -746,7 +770,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E3">
         <v>0.5</v>
@@ -763,7 +787,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -780,7 +804,7 @@
         <v>0.5</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -788,7 +812,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="10" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -797,7 +821,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="10" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20</f>
@@ -824,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" customHeight="1"/>
@@ -836,19 +860,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -862,7 +886,7 @@
         <v>0.9375</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -879,7 +903,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -916,26 +940,59 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:5" ht="39">
+      <c r="A6" s="14">
+        <v>41712</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" customHeight="1">
+      <c r="A7" s="14">
+        <v>41712</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>3.5</v>
+      </c>
+    </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
-        <v>67.5</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -955,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" customHeight="1"/>
@@ -967,41 +1024,108 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1">
+      <c r="A2" s="14">
+        <v>41715</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1">
+      <c r="A3" s="14">
+        <v>41716</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="26">
+      <c r="A4" s="14">
+        <v>41719</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" customHeight="1">
+      <c r="A5" s="14">
+        <v>41720</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
-        <v>67.5</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1033,24 +1157,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1059,15 +1183,14 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>67.5</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1099,24 +1222,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1125,15 +1248,14 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>67.5</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1165,24 +1287,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1191,15 +1313,14 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>67.5</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1231,24 +1352,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1257,15 +1378,14 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>67.5</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1297,24 +1417,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1323,15 +1443,14 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>67.5</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1359,19 +1478,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -1385,7 +1504,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1402,7 +1521,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1410,7 +1529,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1419,7 +1538,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 1'!E21</f>
@@ -1458,19 +1577,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26">
@@ -1484,7 +1603,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1501,7 +1620,7 @@
         <v>0.5</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1509,7 +1628,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1518,7 +1637,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 2'!E21</f>
@@ -1557,19 +1676,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1583,7 +1702,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1600,7 +1719,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E3">
         <v>2.5</v>
@@ -1617,7 +1736,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1634,7 +1753,7 @@
         <v>0.875</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1651,7 +1770,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1659,7 +1778,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1668,7 +1787,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 3'!E21</f>
@@ -1707,19 +1826,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1733,7 +1852,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1750,7 +1869,7 @@
         <v>0.5</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1758,7 +1877,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1767,7 +1886,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 4'!E21</f>
@@ -1806,19 +1925,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -1832,7 +1951,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <v>0.5</v>
@@ -1849,7 +1968,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1866,7 +1985,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1883,7 +2002,7 @@
         <v>0.875</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1900,7 +2019,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1917,7 +2036,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E7">
         <v>2.5</v>
@@ -1934,7 +2053,7 @@
         <v>0.95833333333333337</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -1942,7 +2061,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1951,7 +2070,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 5'!E21</f>
@@ -1990,19 +2109,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -2016,7 +2135,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -2033,7 +2152,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E3">
         <v>1.5</v>
@@ -2050,7 +2169,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2058,7 +2177,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -2067,7 +2186,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 6'!E21</f>
@@ -2107,19 +2226,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="15" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -2133,7 +2252,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -2150,7 +2269,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -2167,7 +2286,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2184,7 +2303,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2201,7 +2320,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -2218,7 +2337,7 @@
         <v>0.22916666666666666</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E7">
         <v>1.5</v>
@@ -2235,7 +2354,7 @@
         <v>0.5</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -2243,7 +2362,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -2252,7 +2371,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 7'!E21</f>
@@ -2260,7 +2379,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2292,19 +2410,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="39">
@@ -2318,7 +2436,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E2">
         <v>2.5</v>
@@ -2335,7 +2453,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -2352,7 +2470,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2369,7 +2487,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -2377,7 +2495,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -2386,7 +2504,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>
@@ -2394,7 +2512,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Submitted timesheet week 12
</commit_message>
<xml_diff>
--- a/Moore-Heather-timesheet.xlsx
+++ b/Moore-Heather-timesheet.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="57">
   <si>
     <t>Compared different online payment services, created databases for laravel, migrated databases, completed ERD, began project description</t>
   </si>
@@ -48,6 +48,10 @@
   </si>
   <si>
     <t>Added login error message to every view, added info to customer orders, worked on adding random suggested products to empty cart page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>First round of usability tests</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -739,19 +743,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26">
@@ -765,7 +769,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -782,7 +786,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3">
         <v>0.5</v>
@@ -799,7 +803,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -816,7 +820,7 @@
         <v>0.5</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -824,7 +828,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -833,7 +837,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <f>E20</f>
@@ -872,19 +876,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -898,7 +902,7 @@
         <v>0.9375</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -915,7 +919,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -932,7 +936,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -949,7 +953,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="39">
@@ -963,7 +967,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -980,7 +984,7 @@
         <v>0.10416666666666667</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E7">
         <v>3.5</v>
@@ -988,7 +992,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -997,7 +1001,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
@@ -1037,19 +1041,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -1063,7 +1067,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2">
         <v>0.5</v>
@@ -1080,7 +1084,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E3">
         <v>2.5</v>
@@ -1097,7 +1101,7 @@
         <v>0.75</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -1114,7 +1118,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1131,7 +1135,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1148,7 +1152,7 @@
         <v>0.5</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1156,7 +1160,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1165,7 +1169,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
@@ -1194,7 +1198,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" customHeight="1"/>
@@ -1205,19 +1209,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="39">
@@ -1237,22 +1241,39 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1">
+      <c r="A3" s="14">
+        <v>41731</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1288,24 +1309,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1314,11 +1335,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1354,24 +1375,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1380,11 +1401,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1420,24 +1441,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1446,11 +1467,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1486,24 +1507,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1512,11 +1533,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1548,19 +1569,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -1574,7 +1595,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1591,7 +1612,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1599,7 +1620,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1608,7 +1629,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <f>E20+'Week 1'!E21</f>
@@ -1616,7 +1637,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1648,19 +1668,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26">
@@ -1674,7 +1694,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1699,7 +1719,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1708,7 +1728,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <f>E20+'Week 2'!E21</f>
@@ -1748,19 +1768,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1808,7 +1828,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1825,7 +1845,7 @@
         <v>0.875</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1842,7 +1862,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1850,7 +1870,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1859,7 +1879,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <f>E20+'Week 3'!E21</f>
@@ -1899,19 +1919,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1925,7 +1945,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1942,7 +1962,7 @@
         <v>0.5</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1950,7 +1970,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1959,7 +1979,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <f>E20+'Week 4'!E21</f>
@@ -1999,19 +2019,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -2025,7 +2045,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E2">
         <v>0.5</v>
@@ -2042,7 +2062,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2059,7 +2079,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2076,7 +2096,7 @@
         <v>0.875</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2093,7 +2113,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -2110,7 +2130,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7">
         <v>2.5</v>
@@ -2127,7 +2147,7 @@
         <v>0.95833333333333337</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -2135,7 +2155,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -2144,7 +2164,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <f>E20+'Week 5'!E21</f>
@@ -2184,19 +2204,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -2210,7 +2230,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -2227,7 +2247,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>1.5</v>
@@ -2244,7 +2264,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2252,7 +2272,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -2261,7 +2281,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <f>E20+'Week 6'!E21</f>
@@ -2302,19 +2322,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -2328,7 +2348,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -2345,7 +2365,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -2362,7 +2382,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2379,7 +2399,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2396,7 +2416,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -2413,7 +2433,7 @@
         <v>0.22916666666666666</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <v>1.5</v>
@@ -2430,7 +2450,7 @@
         <v>0.5</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -2438,7 +2458,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -2447,7 +2467,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <f>E20+'Week 7'!E21</f>
@@ -2487,19 +2507,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="39">
@@ -2513,7 +2533,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <v>2.5</v>
@@ -2530,7 +2550,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -2547,7 +2567,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2564,7 +2584,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -2572,7 +2592,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -2581,7 +2601,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>

</xml_diff>

<commit_message>
Created style guide, submitted 2nd usability tests
</commit_message>
<xml_diff>
--- a/Moore-Heather-timesheet.xlsx
+++ b/Moore-Heather-timesheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="17300" tabRatio="560" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="17300" tabRatio="560" firstSheet="6" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="66">
+  <si>
+    <t>Uploaded product images, created states lookup table, modified table relationships, resolved terminal issue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created dropdown sign in on navbar, adjusted CSS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Compared different online payment services, created databases for laravel, migrated databases, completed ERD, began project description</t>
   </si>
@@ -59,6 +67,156 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Worked on search form and captcha</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Worked on search bar and captcha</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Second usability tests, successfully tested search bar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deployed project to live server, successful live view, adjusted CSS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compiled list of details to get from client</t>
+  </si>
+  <si>
+    <t>Met with client to go over details for website</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created WordPress mockup for peer presentation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Moved WP mockup to live server, prepared for peer presentation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Presented my project idea to the class, got feedback, gave feedback to other students on their projects</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Worked on deleting items from cart and updating cart data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added successful checkout page, successful checkout orders store in database with logged in user relationship</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created and tested view to display all orders of logged in user, added reduce, increase, and remove links on cart view, created view to display user info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created and tested "Add product" page, created admin view to show all products, created "Edit user" button and form, Created and tested "Delete user" button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Successful edit user, edit product, and delete product, created FAQ page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Worked on profile page, created checkout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set up checkout to Stripe, successful test charges from website to Stripe account</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reviewed capstone project timeline, went over rubric, overview of syllabus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brainstormed ideas for Capstone project, setup meeting with website client to discuss details for project</t>
+  </si>
+  <si>
+    <t>Adjusted CSS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Instructor usability test, added sticky fields to forms, added unauthorized access page for users other than admin trying to access admin views</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created sql database dump for alchemortem, created master layout for laravel application</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meet with client to get product info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Photographed and started editing product images</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished editing product images, started master layout and product page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Successful add to cart, view cart, and started on checkout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Worked on restricting admin views from regular users</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added and tested user info update button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adjusted CSS on all pages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added incorrect password error message, created and tested password reset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Worked on CSS and resposiveness</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Worked on product filter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Worked on sort by price filter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finished project description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contacted SiteGround support and adjusted settings to get Laravel project deployed live</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Database presentation with Brenda McFarland, updated Alchemortem database ERD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added foreign keys to tables, migrated tables to db</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Worked on issues with update order status button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Worked on search form</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Sign up auto login, redirects to user account, authorization on guest (cannot view account unless logged in), created cart model to add products to cart</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -118,132 +276,6 @@
     <t>Weekly Total</t>
   </si>
   <si>
-    <t>Created and tested "Add product" page, created admin view to show all products, created "Edit user" button and form, Created and tested "Delete user" button</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Successful edit user, edit product, and delete product, created FAQ page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Worked on profile page, created checkout</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set up checkout to Stripe, successful test charges from website to Stripe account</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reviewed capstone project timeline, went over rubric, overview of syllabus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Brainstormed ideas for Capstone project, setup meeting with website client to discuss details for project</t>
-  </si>
-  <si>
-    <t>Compiled list of details to get from client</t>
-  </si>
-  <si>
-    <t>Met with client to go over details for website</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Created WordPress mockup for peer presentation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Moved WP mockup to live server, prepared for peer presentation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Presented my project idea to the class, got feedback, gave feedback to other students on their projects</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Worked on deleting items from cart and updating cart data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Added successful checkout page, successful checkout orders store in database with logged in user relationship</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Created and tested view to display all orders of logged in user, added reduce, increase, and remove links on cart view, created view to display user info</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Worked on restricting admin views from regular users</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Added and tested user info update button</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Adjusted CSS on all pages</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Added incorrect password error message, created and tested password reset</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Worked on CSS and resposiveness</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Worked on product filter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Worked on sort by price filter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Finished project description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Contacted SiteGround support and adjusted settings to get Laravel project deployed live</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Database presentation with Brenda McFarland, updated Alchemortem database ERD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Added foreign keys to tables, migrated tables to db</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Created sql database dump for alchemortem, created master layout for laravel application</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Meet with client to get product info</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Photographed and started editing product images</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Finished editing product images, started master layout and product page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Successful add to cart, view cart, and started on checkout</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Uploaded product images, created states lookup table, modified table relationships, resolved terminal issue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Created dropdown sign in on navbar, adjusted CSS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Created sign up page, linked page in navigation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -257,6 +289,10 @@
   </si>
   <si>
     <t>Forced user login to checkout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created contact page with form that sends user name, email, and message to the store's email. Successfully tested.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -743,19 +779,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26">
@@ -769,7 +805,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -786,7 +822,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3">
         <v>0.5</v>
@@ -803,7 +839,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -820,7 +856,7 @@
         <v>0.5</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -828,7 +864,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="10" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -837,7 +873,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="10" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E21">
         <f>E20</f>
@@ -845,6 +881,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -876,19 +913,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -902,7 +939,7 @@
         <v>0.9375</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -919,7 +956,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -936,7 +973,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -953,7 +990,7 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="39">
@@ -967,7 +1004,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -984,7 +1021,7 @@
         <v>0.10416666666666667</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E7">
         <v>3.5</v>
@@ -992,7 +1029,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1001,7 +1038,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
@@ -1041,19 +1078,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -1067,7 +1104,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E2">
         <v>0.5</v>
@@ -1084,7 +1121,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E3">
         <v>2.5</v>
@@ -1101,7 +1138,7 @@
         <v>0.75</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -1118,7 +1155,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1135,7 +1172,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1152,7 +1189,7 @@
         <v>0.5</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1160,7 +1197,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1169,7 +1206,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
@@ -1197,7 +1234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1209,19 +1246,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="39">
@@ -1235,7 +1272,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1252,7 +1289,7 @@
         <v>0.5</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1260,7 +1297,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1269,7 +1306,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
@@ -1298,7 +1335,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" customHeight="1"/>
@@ -1309,37 +1346,105 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="39">
+      <c r="A2" s="14">
+        <v>41738</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="26">
+      <c r="A3" s="14">
+        <v>41738</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C3" s="6">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1">
+      <c r="A4" s="14">
+        <v>41739</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="39">
+      <c r="A5" s="14">
+        <v>41740</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>91</v>
+        <v>101.5</v>
       </c>
     </row>
   </sheetData>
@@ -1364,7 +1469,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" customHeight="1"/>
@@ -1375,37 +1480,88 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1">
+      <c r="A2" s="14">
+        <v>41745</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1">
+      <c r="A3" s="14">
+        <v>41747</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1">
+      <c r="A4" s="14">
+        <v>41747</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.8125</v>
+      </c>
+      <c r="C4" s="6">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>91</v>
+        <v>110.5</v>
       </c>
     </row>
   </sheetData>
@@ -1429,8 +1585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" customHeight="1"/>
@@ -1441,37 +1597,71 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1">
+      <c r="A2" s="14">
+        <v>41751</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1">
+      <c r="A3" s="14">
+        <v>41752</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>91</v>
+        <v>114.5</v>
       </c>
     </row>
   </sheetData>
@@ -1507,24 +1697,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1533,11 +1723,11 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>91</v>
+        <v>110.5</v>
       </c>
     </row>
   </sheetData>
@@ -1569,19 +1759,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -1595,7 +1785,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1612,7 +1802,7 @@
         <v>0.91666666666666663</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1620,7 +1810,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1629,7 +1819,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E21">
         <f>E20+'Week 1'!E21</f>
@@ -1637,6 +1827,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1668,19 +1859,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26">
@@ -1694,7 +1885,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1711,7 +1902,7 @@
         <v>0.5</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1719,7 +1910,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1728,7 +1919,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E21">
         <f>E20+'Week 2'!E21</f>
@@ -1768,19 +1959,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1794,7 +1985,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1811,7 +2002,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <v>2.5</v>
@@ -1828,7 +2019,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1845,7 +2036,7 @@
         <v>0.875</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1862,7 +2053,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1870,7 +2061,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1879,7 +2070,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E21">
         <f>E20+'Week 3'!E21</f>
@@ -1919,19 +2110,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1945,7 +2136,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1962,7 +2153,7 @@
         <v>0.5</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1970,7 +2161,7 @@
     </row>
     <row r="20" spans="4:5">
       <c r="D20" s="4" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -1979,7 +2170,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" s="4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E21">
         <f>E20+'Week 4'!E21</f>
@@ -2019,19 +2210,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -2045,7 +2236,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="E2">
         <v>0.5</v>
@@ -2062,7 +2253,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2079,7 +2270,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2096,7 +2287,7 @@
         <v>0.875</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2113,7 +2304,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -2130,7 +2321,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E7">
         <v>2.5</v>
@@ -2147,7 +2338,7 @@
         <v>0.95833333333333337</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -2155,7 +2346,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -2164,7 +2355,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E21">
         <f>E20+'Week 5'!E21</f>
@@ -2204,19 +2395,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -2230,7 +2421,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -2247,7 +2438,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="E3">
         <v>1.5</v>
@@ -2264,7 +2455,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2272,7 +2463,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -2281,7 +2472,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E21">
         <f>E20+'Week 6'!E21</f>
@@ -2322,19 +2513,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="15" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
@@ -2348,7 +2539,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -2365,7 +2556,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -2382,7 +2573,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2399,7 +2590,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2416,7 +2607,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -2433,7 +2624,7 @@
         <v>0.22916666666666666</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="E7">
         <v>1.5</v>
@@ -2450,7 +2641,7 @@
         <v>0.5</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -2458,7 +2649,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -2467,7 +2658,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E21">
         <f>E20+'Week 7'!E21</f>
@@ -2507,19 +2698,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="39">
@@ -2533,7 +2724,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2">
         <v>2.5</v>
@@ -2550,7 +2741,7 @@
         <v>0.77083333333333337</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -2567,7 +2758,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2584,7 +2775,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -2592,7 +2783,7 @@
     </row>
     <row r="20" spans="4:5" ht="18" customHeight="1">
       <c r="D20" s="4" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="E20">
         <f>SUM(E2:E19)</f>
@@ -2601,7 +2792,7 @@
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1">
       <c r="D21" s="4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>

</xml_diff>